<commit_message>
GRCW-575, Added Font Sizes by Grade Type
</commit_message>
<xml_diff>
--- a/pdf/RTTBC23-Heat-Map.xlsx
+++ b/pdf/RTTBC23-Heat-Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="805" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04710C85-6B24-4FDA-AAB8-D1C4254009E8}"/>
+  <xr:revisionPtr revIDLastSave="872" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{930E4CCC-6486-4DE1-89F4-11E23288DA7C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -396,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +424,54 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -582,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,19 +663,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -637,15 +673,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -658,10 +685,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,15 +727,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,13 +736,106 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,123 +1166,123 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13"/>
+      <c r="B1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="45" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="23"/>
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="2" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="25"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+    <row r="6" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
         <v>2</v>
       </c>
       <c r="B6" s="5"/>
@@ -1172,13 +1292,13 @@
       <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="46" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+      <c r="A7" s="15">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1193,44 +1313,44 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
+    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
         <v>4</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="44" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="43" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="26">
+      <c r="A10" s="19">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1239,44 +1359,44 @@
       <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="44" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="2" t="s">
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="24"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="25"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
+      <c r="A13" s="15">
         <v>6</v>
       </c>
       <c r="B13" s="5"/>
@@ -1291,290 +1411,290 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="26">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="19">
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="44" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="15" t="s">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="23"/>
+      <c r="B15" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="3" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="23"/>
+      <c r="B18" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="2" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
+    <row r="19" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="20"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="16" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="54" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="26">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="19">
         <v>9</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="44" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="44" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="24"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="26">
+      <c r="C22" s="42"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
         <v>10</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="3" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="26">
+      <c r="A25" s="19">
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="26">
+      <c r="C26" s="57"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="19">
         <v>12</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="3" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
-      <c r="B28" s="2" t="s">
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="23"/>
+      <c r="B28" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="2" t="s">
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="44" t="s">
         <v>64</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="24"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="16" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="58" t="s">
         <v>68</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="26">
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="19">
         <v>13</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="44" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="16" t="s">
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="20"/>
+      <c r="B31" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="19">
+      <c r="C31" s="22"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="15">
         <v>14</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="62" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="6"/>
@@ -1582,7 +1702,7 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19">
+      <c r="A33" s="15">
         <v>15</v>
       </c>
       <c r="B33" s="6"/>
@@ -1599,170 +1719,170 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="26">
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="19">
         <v>16</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="44"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="44" t="s">
+      <c r="D34" s="21"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="44" t="s">
+      <c r="H34" s="48" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="45"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="52"/>
     </row>
     <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="26">
+      <c r="D36" s="22"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="49"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19">
         <v>17</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="41" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="34" t="s">
         <v>94</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="67" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
-      <c r="B38" s="15" t="s">
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="23"/>
+      <c r="B38" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="2" t="s">
+      <c r="C38" s="64"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="53" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
-      <c r="B39" s="2" t="s">
+    <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
+      <c r="B39" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="15" t="s">
+      <c r="C39" s="64"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="66" t="s">
         <v>91</v>
       </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="43"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="26">
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="19">
         <v>18</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="16"/>
+      <c r="C41" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="20" t="s">
+      <c r="F41" s="16"/>
+      <c r="G41" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="68" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="15" t="s">
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="23"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
-      <c r="B43" s="25"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+    </row>
+    <row r="43" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="20"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="19">
+      <c r="F43" s="18"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+    </row>
+    <row r="44" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="15">
         <v>20</v>
       </c>
       <c r="B44" s="6"/>
@@ -1770,71 +1890,67 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="46" t="s">
         <v>108</v>
       </c>
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="32" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="34"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
     <mergeCell ref="H30:H31"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="A25:A26"/>
@@ -1851,36 +1967,40 @@
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="A30:A31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>